<commit_message>
update malaria.xlsx with latest data
</commit_message>
<xml_diff>
--- a/malaria.xlsx
+++ b/malaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Bageshwar"/>
@@ -17768,7 +17768,7 @@
   </sheetPr>
   <dimension ref="A1:EO12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28109,7 +28109,7 @@
   </sheetPr>
   <dimension ref="A1:EO12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Update malaria data in Excel file
</commit_message>
<xml_diff>
--- a/malaria.xlsx
+++ b/malaria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Bageshwar"/>
@@ -28109,7 +28109,7 @@
   </sheetPr>
   <dimension ref="A1:EO12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -35003,11 +35003,11 @@
   </sheetPr>
   <dimension ref="A1:EO12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="35.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="77.14785714285713" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>

</xml_diff>